<commit_message>
working on expense report
</commit_message>
<xml_diff>
--- a/application/plugins/Reports_summary_expense/views/Reports_summary_expense.xlsx
+++ b/application/plugins/Reports_summary_expense/views/Reports_summary_expense.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1356" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="1350" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Отчет" sheetId="1" r:id="rId1"/>
@@ -70,9 +70,6 @@
     <t>{$v-&gt;rows[]-&gt;company_name}</t>
   </si>
   <si>
-    <t>{$v-&gt;rows[]-&gt;expense_label}</t>
-  </si>
-  <si>
     <t>{$v-&gt;rows[]-&gt;trans_name}</t>
   </si>
   <si>
@@ -83,6 +80,9 @@
   </si>
   <si>
     <t>{$v-&gt;totals[]-&gt;expense_label}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;label}</t>
   </si>
 </sst>
 </file>
@@ -435,6 +435,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -473,9 +476,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -538,7 +538,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -573,7 +573,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -785,35 +785,35 @@
   <dimension ref="B1:H11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.21875" customWidth="1"/>
-    <col min="2" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" customWidth="1"/>
-    <col min="7" max="7" width="61.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="7" width="61.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D2" s="19" t="s">
+    <row r="1" spans="2:8" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="22"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D3" s="25" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="26"/>
+      <c r="E3" s="27"/>
       <c r="F3" s="11" t="s">
         <v>11</v>
       </c>
@@ -824,57 +824,57 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D4" s="22" t="s">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D5" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="28"/>
+    <row r="5" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="D5" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="29"/>
       <c r="F5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D6" s="1"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
+    <row r="7" spans="2:8" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="29" t="s">
-        <v>20</v>
+      <c r="C9" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>6</v>
@@ -892,12 +892,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>19</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>17</v>
@@ -915,7 +915,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>

</xml_diff>